<commit_message>
Print Lagi Absent Juni2024
</commit_message>
<xml_diff>
--- a/ABSENSI LANDO 2024.xlsx
+++ b/ABSENSI LANDO 2024.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="13545" windowHeight="12375"/>
+    <workbookView windowWidth="27945" windowHeight="12375"/>
   </bookViews>
   <sheets>
     <sheet name="sheet 1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'sheet 1'!$A$2:$AI$26</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'sheet 1'!$A$1:$AI$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'sheet 1'!$A$2:$AI$27</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'sheet 1'!$A$1:$AI$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
   <si>
     <t>DAFTAR HADIR (LANDO)</t>
   </si>
@@ -48,195 +48,105 @@
     <t>BAGIAN</t>
   </si>
   <si>
-    <t>PERIODE 1 s/d 30 APRIL 2024</t>
-  </si>
-  <si>
-    <t>LD-01</t>
-  </si>
-  <si>
-    <t>TONDI MULYADI HASIBUAN</t>
+    <t>PERIODE 1 s/d 30 Juni 2024</t>
+  </si>
+  <si>
+    <t>LD-02</t>
+  </si>
+  <si>
+    <t>DIDIK TRI</t>
+  </si>
+  <si>
+    <t>WELDER/焊工</t>
+  </si>
+  <si>
+    <t>LD-05</t>
+  </si>
+  <si>
+    <t>MARIO</t>
+  </si>
+  <si>
+    <t>HELPER/小工</t>
+  </si>
+  <si>
+    <t>LD-06</t>
+  </si>
+  <si>
+    <t>RAMLAN</t>
+  </si>
+  <si>
+    <t>SCAFFOLD/脚手架工</t>
+  </si>
+  <si>
+    <t>LD-07</t>
+  </si>
+  <si>
+    <t>AGUNG</t>
+  </si>
+  <si>
+    <t>LD-09</t>
+  </si>
+  <si>
+    <t>YANSPIT</t>
+  </si>
+  <si>
+    <t>LD-10</t>
+  </si>
+  <si>
+    <t>ANDRIS</t>
+  </si>
+  <si>
+    <t>LD-14</t>
+  </si>
+  <si>
+    <t>FETRI</t>
+  </si>
+  <si>
+    <t>LD-16</t>
+  </si>
+  <si>
+    <t>RIZKY</t>
+  </si>
+  <si>
+    <t>LD-19</t>
+  </si>
+  <si>
+    <t>STEVEN</t>
+  </si>
+  <si>
+    <t>LD-23</t>
+  </si>
+  <si>
+    <t>SALIM</t>
   </si>
   <si>
     <r>
       <rPr>
         <sz val="10"/>
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <charset val="0"/>
       </rPr>
-      <t>WELDER/</t>
+      <t>FITTER I/</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="0"/>
-      </rPr>
-      <t>焊工</t>
-    </r>
-  </si>
-  <si>
-    <t>LD-03</t>
-  </si>
-  <si>
-    <t>ADENG HIDAYAT</t>
-  </si>
-  <si>
-    <t>LD-05</t>
-  </si>
-  <si>
-    <t>MARION DEVIDS PAPARANG</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Arial"/>
-        <charset val="0"/>
-      </rPr>
-      <t>HELPER/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="0"/>
-      </rPr>
-      <t>小工</t>
-    </r>
-  </si>
-  <si>
-    <t>LD-06</t>
-  </si>
-  <si>
-    <t>RAMLAN</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Arial"/>
-        <charset val="0"/>
-      </rPr>
-      <t>SCAFFOLDER/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="0"/>
-      </rPr>
-      <t>脚手架工</t>
-    </r>
-  </si>
-  <si>
-    <t>LD-10</t>
-  </si>
-  <si>
-    <t>ANDRIS SELANNO</t>
-  </si>
-  <si>
-    <t>LD-12</t>
-  </si>
-  <si>
-    <t>YAMES TODOM</t>
-  </si>
-  <si>
-    <t>LD-14</t>
-  </si>
-  <si>
-    <t>FETRI</t>
-  </si>
-  <si>
-    <t>WELDER/焊工</t>
-  </si>
-  <si>
-    <t>LD-15</t>
-  </si>
-  <si>
-    <t>ZICO MANUSAMA</t>
-  </si>
-  <si>
-    <t>LD-16</t>
-  </si>
-  <si>
-    <t>RIZKY SENTINUWO</t>
-  </si>
-  <si>
-    <t>HELPER/小工</t>
-  </si>
-  <si>
-    <t>LD-17</t>
-  </si>
-  <si>
-    <t>ROBI SURE</t>
-  </si>
-  <si>
-    <t>LD-19</t>
-  </si>
-  <si>
-    <t>STEFEN NGONGARE</t>
-  </si>
-  <si>
-    <t>LD-21</t>
-  </si>
-  <si>
-    <t>AHMAD RIZKY</t>
-  </si>
-  <si>
-    <t>LD-23</t>
-  </si>
-  <si>
-    <t>SALIM PUTRA ADE</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Arial"/>
-        <charset val="0"/>
-      </rPr>
-      <t>FITTER/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
+        <color rgb="FF000000"/>
+        <rFont val="SimSun"/>
         <charset val="0"/>
       </rPr>
       <t>安装工</t>
     </r>
   </si>
   <si>
-    <t>LD-28</t>
-  </si>
-  <si>
-    <t>MARSON HOROHIUNG</t>
-  </si>
-  <si>
-    <t>LD-32</t>
-  </si>
-  <si>
-    <t>INDRA GUNAWAN</t>
-  </si>
-  <si>
-    <t>LD-36</t>
-  </si>
-  <si>
-    <t>PARLEUS</t>
-  </si>
-  <si>
-    <t>LD-38</t>
-  </si>
-  <si>
-    <t>WELSON</t>
+    <t>LD-25</t>
+  </si>
+  <si>
+    <t>JUMADI</t>
+  </si>
+  <si>
+    <t>FITTER I/安装工</t>
   </si>
   <si>
     <t>LD-39</t>
@@ -245,46 +155,70 @@
     <t>SABRI</t>
   </si>
   <si>
+    <t>LD-41</t>
+  </si>
+  <si>
+    <t>AMON</t>
+  </si>
+  <si>
+    <t>LD-44</t>
+  </si>
+  <si>
+    <t>AZAM</t>
+  </si>
+  <si>
     <t>LD-46</t>
   </si>
   <si>
-    <t>REVIAN SENTINUWO</t>
-  </si>
-  <si>
-    <t>LD-49</t>
-  </si>
-  <si>
-    <t>ANTONIUS PANGENDAHEN</t>
-  </si>
-  <si>
-    <t>LD-51</t>
-  </si>
-  <si>
-    <t>SOLIDEO BATARIA</t>
+    <t>VIAN</t>
+  </si>
+  <si>
+    <t>LD-50</t>
+  </si>
+  <si>
+    <t>OVER BATOK</t>
   </si>
   <si>
     <t>LD-55</t>
   </si>
   <si>
-    <t>ALENG GUNAWAN</t>
-  </si>
-  <si>
-    <t>LD-58</t>
+    <t>M ALWI</t>
+  </si>
+  <si>
+    <t>LD-59</t>
   </si>
   <si>
     <t>ALTER HODJA</t>
   </si>
   <si>
-    <t>LD-59</t>
-  </si>
-  <si>
-    <t>PETRUS TOUDJOUNG</t>
-  </si>
-  <si>
     <t>LD-62</t>
   </si>
   <si>
-    <t>MULKAN MALAWAT</t>
+    <t>MULKAM</t>
+  </si>
+  <si>
+    <t>LD-66</t>
+  </si>
+  <si>
+    <t>SAIFUL AMIN</t>
+  </si>
+  <si>
+    <t>LD-77</t>
+  </si>
+  <si>
+    <t>TAUFIK</t>
+  </si>
+  <si>
+    <t>LD-88</t>
+  </si>
+  <si>
+    <t>ADRI</t>
+  </si>
+  <si>
+    <t>LD-99</t>
+  </si>
+  <si>
+    <t>SANIN</t>
   </si>
 </sst>
 </file>
@@ -297,7 +231,7 @@
     <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="32">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -365,6 +299,12 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <charset val="0"/>
     </font>
@@ -514,17 +454,23 @@
     </font>
     <font>
       <sz val="10"/>
-      <color indexed="8"/>
-      <name val="宋体"/>
+      <color rgb="FF000000"/>
+      <name val="SimSun"/>
       <charset val="0"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -854,55 +800,52 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -917,74 +860,77 @@
     <xf numFmtId="0" fontId="29" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1024,11 +970,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1349,10 +1301,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AI36"/>
+  <dimension ref="A1:AI27"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.75" defaultRowHeight="12.75"/>
@@ -1610,28 +1562,28 @@
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
       <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="13"/>
-      <c r="S5" s="13"/>
-      <c r="T5" s="13"/>
-      <c r="U5" s="13"/>
-      <c r="V5" s="13"/>
-      <c r="W5" s="13"/>
-      <c r="X5" s="13"/>
-      <c r="Y5" s="13"/>
-      <c r="Z5" s="13"/>
-      <c r="AA5" s="13"/>
-      <c r="AB5" s="13"/>
-      <c r="AC5" s="13"/>
-      <c r="AD5" s="13"/>
-      <c r="AE5" s="13"/>
-      <c r="AF5" s="13"/>
-      <c r="AG5" s="13"/>
-      <c r="AH5" s="13"/>
-      <c r="AI5" s="13"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="16"/>
+      <c r="V5" s="16"/>
+      <c r="W5" s="16"/>
+      <c r="X5" s="16"/>
+      <c r="Y5" s="16"/>
+      <c r="Z5" s="16"/>
+      <c r="AA5" s="16"/>
+      <c r="AB5" s="16"/>
+      <c r="AC5" s="16"/>
+      <c r="AD5" s="16"/>
+      <c r="AE5" s="16"/>
+      <c r="AF5" s="16"/>
+      <c r="AG5" s="16"/>
+      <c r="AH5" s="16"/>
+      <c r="AI5" s="16"/>
     </row>
     <row r="6" s="3" customFormat="1" ht="14" customHeight="1" spans="1:35">
       <c r="A6" s="9">
@@ -1644,7 +1596,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
@@ -1655,41 +1607,41 @@
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="13"/>
-      <c r="S6" s="13"/>
-      <c r="T6" s="13"/>
-      <c r="U6" s="13"/>
-      <c r="V6" s="13"/>
-      <c r="W6" s="13"/>
-      <c r="X6" s="13"/>
-      <c r="Y6" s="13"/>
-      <c r="Z6" s="13"/>
-      <c r="AA6" s="13"/>
-      <c r="AB6" s="13"/>
-      <c r="AC6" s="13"/>
-      <c r="AD6" s="13"/>
-      <c r="AE6" s="13"/>
-      <c r="AF6" s="13"/>
-      <c r="AG6" s="13"/>
-      <c r="AH6" s="13"/>
-      <c r="AI6" s="13"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="16"/>
+      <c r="W6" s="16"/>
+      <c r="X6" s="16"/>
+      <c r="Y6" s="16"/>
+      <c r="Z6" s="16"/>
+      <c r="AA6" s="16"/>
+      <c r="AB6" s="16"/>
+      <c r="AC6" s="16"/>
+      <c r="AD6" s="16"/>
+      <c r="AE6" s="16"/>
+      <c r="AF6" s="16"/>
+      <c r="AG6" s="16"/>
+      <c r="AH6" s="16"/>
+      <c r="AI6" s="16"/>
     </row>
     <row r="7" s="3" customFormat="1" ht="14" customHeight="1" spans="1:35">
       <c r="A7" s="9">
         <v>3</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
@@ -1700,41 +1652,41 @@
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
       <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="13"/>
-      <c r="S7" s="13"/>
-      <c r="T7" s="13"/>
-      <c r="U7" s="13"/>
-      <c r="V7" s="13"/>
-      <c r="W7" s="13"/>
-      <c r="X7" s="13"/>
-      <c r="Y7" s="13"/>
-      <c r="Z7" s="13"/>
-      <c r="AA7" s="13"/>
-      <c r="AB7" s="13"/>
-      <c r="AC7" s="13"/>
-      <c r="AD7" s="13"/>
-      <c r="AE7" s="13"/>
-      <c r="AF7" s="13"/>
-      <c r="AG7" s="13"/>
-      <c r="AH7" s="13"/>
-      <c r="AI7" s="13"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="16"/>
+      <c r="S7" s="16"/>
+      <c r="T7" s="16"/>
+      <c r="U7" s="16"/>
+      <c r="V7" s="16"/>
+      <c r="W7" s="16"/>
+      <c r="X7" s="16"/>
+      <c r="Y7" s="16"/>
+      <c r="Z7" s="16"/>
+      <c r="AA7" s="16"/>
+      <c r="AB7" s="16"/>
+      <c r="AC7" s="16"/>
+      <c r="AD7" s="16"/>
+      <c r="AE7" s="16"/>
+      <c r="AF7" s="16"/>
+      <c r="AG7" s="16"/>
+      <c r="AH7" s="16"/>
+      <c r="AI7" s="16"/>
     </row>
     <row r="8" s="3" customFormat="1" ht="14" customHeight="1" spans="1:35">
       <c r="A8" s="9">
         <v>4</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
@@ -1745,28 +1697,28 @@
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
       <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="13"/>
-      <c r="S8" s="13"/>
-      <c r="T8" s="13"/>
-      <c r="U8" s="13"/>
-      <c r="V8" s="13"/>
-      <c r="W8" s="13"/>
-      <c r="X8" s="13"/>
-      <c r="Y8" s="13"/>
-      <c r="Z8" s="13"/>
-      <c r="AA8" s="13"/>
-      <c r="AB8" s="13"/>
-      <c r="AC8" s="13"/>
-      <c r="AD8" s="13"/>
-      <c r="AE8" s="13"/>
-      <c r="AF8" s="13"/>
-      <c r="AG8" s="13"/>
-      <c r="AH8" s="13"/>
-      <c r="AI8" s="13"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="16"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="16"/>
+      <c r="V8" s="16"/>
+      <c r="W8" s="16"/>
+      <c r="X8" s="16"/>
+      <c r="Y8" s="16"/>
+      <c r="Z8" s="16"/>
+      <c r="AA8" s="16"/>
+      <c r="AB8" s="16"/>
+      <c r="AC8" s="16"/>
+      <c r="AD8" s="16"/>
+      <c r="AE8" s="16"/>
+      <c r="AF8" s="16"/>
+      <c r="AG8" s="16"/>
+      <c r="AH8" s="16"/>
+      <c r="AI8" s="16"/>
     </row>
     <row r="9" s="3" customFormat="1" ht="14" customHeight="1" spans="1:35">
       <c r="A9" s="9">
@@ -1779,7 +1731,7 @@
         <v>18</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
@@ -1790,28 +1742,28 @@
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
       <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="13"/>
-      <c r="R9" s="13"/>
-      <c r="S9" s="13"/>
-      <c r="T9" s="13"/>
-      <c r="U9" s="13"/>
-      <c r="V9" s="13"/>
-      <c r="W9" s="13"/>
-      <c r="X9" s="13"/>
-      <c r="Y9" s="13"/>
-      <c r="Z9" s="13"/>
-      <c r="AA9" s="13"/>
-      <c r="AB9" s="13"/>
-      <c r="AC9" s="13"/>
-      <c r="AD9" s="13"/>
-      <c r="AE9" s="13"/>
-      <c r="AF9" s="13"/>
-      <c r="AG9" s="13"/>
-      <c r="AH9" s="13"/>
-      <c r="AI9" s="13"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16"/>
+      <c r="T9" s="16"/>
+      <c r="U9" s="16"/>
+      <c r="V9" s="16"/>
+      <c r="W9" s="16"/>
+      <c r="X9" s="16"/>
+      <c r="Y9" s="16"/>
+      <c r="Z9" s="16"/>
+      <c r="AA9" s="16"/>
+      <c r="AB9" s="16"/>
+      <c r="AC9" s="16"/>
+      <c r="AD9" s="16"/>
+      <c r="AE9" s="16"/>
+      <c r="AF9" s="16"/>
+      <c r="AG9" s="16"/>
+      <c r="AH9" s="16"/>
+      <c r="AI9" s="16"/>
     </row>
     <row r="10" s="3" customFormat="1" ht="14" customHeight="1" spans="1:35">
       <c r="A10" s="9">
@@ -1824,7 +1776,7 @@
         <v>20</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
@@ -1835,28 +1787,28 @@
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
       <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="13"/>
-      <c r="S10" s="13"/>
-      <c r="T10" s="13"/>
-      <c r="U10" s="13"/>
-      <c r="V10" s="13"/>
-      <c r="W10" s="13"/>
-      <c r="X10" s="13"/>
-      <c r="Y10" s="13"/>
-      <c r="Z10" s="13"/>
-      <c r="AA10" s="13"/>
-      <c r="AB10" s="13"/>
-      <c r="AC10" s="13"/>
-      <c r="AD10" s="13"/>
-      <c r="AE10" s="13"/>
-      <c r="AF10" s="13"/>
-      <c r="AG10" s="13"/>
-      <c r="AH10" s="13"/>
-      <c r="AI10" s="13"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="16"/>
+      <c r="S10" s="16"/>
+      <c r="T10" s="16"/>
+      <c r="U10" s="16"/>
+      <c r="V10" s="16"/>
+      <c r="W10" s="16"/>
+      <c r="X10" s="16"/>
+      <c r="Y10" s="16"/>
+      <c r="Z10" s="16"/>
+      <c r="AA10" s="16"/>
+      <c r="AB10" s="16"/>
+      <c r="AC10" s="16"/>
+      <c r="AD10" s="16"/>
+      <c r="AE10" s="16"/>
+      <c r="AF10" s="16"/>
+      <c r="AG10" s="16"/>
+      <c r="AH10" s="16"/>
+      <c r="AI10" s="16"/>
     </row>
     <row r="11" s="3" customFormat="1" ht="14" customHeight="1" spans="1:35">
       <c r="A11" s="9">
@@ -1869,7 +1821,7 @@
         <v>22</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
@@ -1880,41 +1832,41 @@
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
       <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="13"/>
-      <c r="R11" s="13"/>
-      <c r="S11" s="13"/>
-      <c r="T11" s="13"/>
-      <c r="U11" s="13"/>
-      <c r="V11" s="13"/>
-      <c r="W11" s="13"/>
-      <c r="X11" s="13"/>
-      <c r="Y11" s="13"/>
-      <c r="Z11" s="13"/>
-      <c r="AA11" s="13"/>
-      <c r="AB11" s="13"/>
-      <c r="AC11" s="13"/>
-      <c r="AD11" s="13"/>
-      <c r="AE11" s="13"/>
-      <c r="AF11" s="13"/>
-      <c r="AG11" s="13"/>
-      <c r="AH11" s="13"/>
-      <c r="AI11" s="13"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="16"/>
+      <c r="T11" s="16"/>
+      <c r="U11" s="16"/>
+      <c r="V11" s="16"/>
+      <c r="W11" s="16"/>
+      <c r="X11" s="16"/>
+      <c r="Y11" s="16"/>
+      <c r="Z11" s="16"/>
+      <c r="AA11" s="16"/>
+      <c r="AB11" s="16"/>
+      <c r="AC11" s="16"/>
+      <c r="AD11" s="16"/>
+      <c r="AE11" s="16"/>
+      <c r="AF11" s="16"/>
+      <c r="AG11" s="16"/>
+      <c r="AH11" s="16"/>
+      <c r="AI11" s="16"/>
     </row>
     <row r="12" s="3" customFormat="1" ht="14" customHeight="1" spans="1:35">
       <c r="A12" s="9">
         <v>8</v>
       </c>
       <c r="B12" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="14" t="s">
-        <v>25</v>
-      </c>
       <c r="D12" s="12" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
@@ -1925,41 +1877,41 @@
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
       <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="13"/>
-      <c r="R12" s="13"/>
-      <c r="S12" s="13"/>
-      <c r="T12" s="13"/>
-      <c r="U12" s="13"/>
-      <c r="V12" s="13"/>
-      <c r="W12" s="13"/>
-      <c r="X12" s="13"/>
-      <c r="Y12" s="13"/>
-      <c r="Z12" s="13"/>
-      <c r="AA12" s="13"/>
-      <c r="AB12" s="13"/>
-      <c r="AC12" s="13"/>
-      <c r="AD12" s="13"/>
-      <c r="AE12" s="13"/>
-      <c r="AF12" s="13"/>
-      <c r="AG12" s="13"/>
-      <c r="AH12" s="13"/>
-      <c r="AI12" s="13"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
+      <c r="S12" s="16"/>
+      <c r="T12" s="16"/>
+      <c r="U12" s="16"/>
+      <c r="V12" s="16"/>
+      <c r="W12" s="16"/>
+      <c r="X12" s="16"/>
+      <c r="Y12" s="16"/>
+      <c r="Z12" s="16"/>
+      <c r="AA12" s="16"/>
+      <c r="AB12" s="16"/>
+      <c r="AC12" s="16"/>
+      <c r="AD12" s="16"/>
+      <c r="AE12" s="16"/>
+      <c r="AF12" s="16"/>
+      <c r="AG12" s="16"/>
+      <c r="AH12" s="16"/>
+      <c r="AI12" s="16"/>
     </row>
     <row r="13" s="3" customFormat="1" ht="14" customHeight="1" spans="1:35">
       <c r="A13" s="9">
         <v>9</v>
       </c>
       <c r="B13" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>27</v>
-      </c>
       <c r="D13" s="12" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
@@ -1970,41 +1922,41 @@
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
       <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="13"/>
-      <c r="R13" s="13"/>
-      <c r="S13" s="13"/>
-      <c r="T13" s="13"/>
-      <c r="U13" s="13"/>
-      <c r="V13" s="13"/>
-      <c r="W13" s="13"/>
-      <c r="X13" s="13"/>
-      <c r="Y13" s="13"/>
-      <c r="Z13" s="13"/>
-      <c r="AA13" s="13"/>
-      <c r="AB13" s="13"/>
-      <c r="AC13" s="13"/>
-      <c r="AD13" s="13"/>
-      <c r="AE13" s="13"/>
-      <c r="AF13" s="13"/>
-      <c r="AG13" s="13"/>
-      <c r="AH13" s="13"/>
-      <c r="AI13" s="13"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="16"/>
+      <c r="S13" s="16"/>
+      <c r="T13" s="16"/>
+      <c r="U13" s="16"/>
+      <c r="V13" s="16"/>
+      <c r="W13" s="16"/>
+      <c r="X13" s="16"/>
+      <c r="Y13" s="16"/>
+      <c r="Z13" s="16"/>
+      <c r="AA13" s="16"/>
+      <c r="AB13" s="16"/>
+      <c r="AC13" s="16"/>
+      <c r="AD13" s="16"/>
+      <c r="AE13" s="16"/>
+      <c r="AF13" s="16"/>
+      <c r="AG13" s="16"/>
+      <c r="AH13" s="16"/>
+      <c r="AI13" s="16"/>
     </row>
     <row r="14" spans="1:35">
       <c r="A14" s="9">
         <v>10</v>
       </c>
       <c r="B14" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="15" t="s">
         <v>29</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>13</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
@@ -2015,41 +1967,41 @@
       <c r="K14" s="13"/>
       <c r="L14" s="13"/>
       <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="13"/>
-      <c r="R14" s="13"/>
-      <c r="S14" s="13"/>
-      <c r="T14" s="13"/>
-      <c r="U14" s="13"/>
-      <c r="V14" s="13"/>
-      <c r="W14" s="13"/>
-      <c r="X14" s="13"/>
-      <c r="Y14" s="13"/>
-      <c r="Z14" s="13"/>
-      <c r="AA14" s="13"/>
-      <c r="AB14" s="13"/>
-      <c r="AC14" s="13"/>
-      <c r="AD14" s="13"/>
-      <c r="AE14" s="13"/>
-      <c r="AF14" s="13"/>
-      <c r="AG14" s="13"/>
-      <c r="AH14" s="13"/>
-      <c r="AI14" s="13"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="16"/>
+      <c r="S14" s="16"/>
+      <c r="T14" s="16"/>
+      <c r="U14" s="16"/>
+      <c r="V14" s="16"/>
+      <c r="W14" s="16"/>
+      <c r="X14" s="16"/>
+      <c r="Y14" s="16"/>
+      <c r="Z14" s="16"/>
+      <c r="AA14" s="16"/>
+      <c r="AB14" s="16"/>
+      <c r="AC14" s="16"/>
+      <c r="AD14" s="16"/>
+      <c r="AE14" s="16"/>
+      <c r="AF14" s="16"/>
+      <c r="AG14" s="16"/>
+      <c r="AH14" s="16"/>
+      <c r="AI14" s="16"/>
     </row>
     <row r="15" s="3" customFormat="1" ht="14" customHeight="1" spans="1:35">
       <c r="A15" s="9">
         <v>11</v>
       </c>
       <c r="B15" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="D15" s="12" t="s">
         <v>32</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>13</v>
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
@@ -2060,28 +2012,28 @@
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
       <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="13"/>
-      <c r="R15" s="13"/>
-      <c r="S15" s="13"/>
-      <c r="T15" s="13"/>
-      <c r="U15" s="13"/>
-      <c r="V15" s="13"/>
-      <c r="W15" s="13"/>
-      <c r="X15" s="13"/>
-      <c r="Y15" s="13"/>
-      <c r="Z15" s="13"/>
-      <c r="AA15" s="13"/>
-      <c r="AB15" s="13"/>
-      <c r="AC15" s="13"/>
-      <c r="AD15" s="13"/>
-      <c r="AE15" s="13"/>
-      <c r="AF15" s="13"/>
-      <c r="AG15" s="13"/>
-      <c r="AH15" s="13"/>
-      <c r="AI15" s="13"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="16"/>
+      <c r="S15" s="16"/>
+      <c r="T15" s="16"/>
+      <c r="U15" s="16"/>
+      <c r="V15" s="16"/>
+      <c r="W15" s="16"/>
+      <c r="X15" s="16"/>
+      <c r="Y15" s="16"/>
+      <c r="Z15" s="16"/>
+      <c r="AA15" s="16"/>
+      <c r="AB15" s="16"/>
+      <c r="AC15" s="16"/>
+      <c r="AD15" s="16"/>
+      <c r="AE15" s="16"/>
+      <c r="AF15" s="16"/>
+      <c r="AG15" s="16"/>
+      <c r="AH15" s="16"/>
+      <c r="AI15" s="16"/>
     </row>
     <row r="16" s="3" customFormat="1" ht="14" customHeight="1" spans="1:35">
       <c r="A16" s="9">
@@ -2094,7 +2046,7 @@
         <v>34</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
@@ -2105,28 +2057,28 @@
       <c r="K16" s="13"/>
       <c r="L16" s="13"/>
       <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="13"/>
-      <c r="P16" s="13"/>
-      <c r="Q16" s="13"/>
-      <c r="R16" s="13"/>
-      <c r="S16" s="13"/>
-      <c r="T16" s="13"/>
-      <c r="U16" s="13"/>
-      <c r="V16" s="13"/>
-      <c r="W16" s="13"/>
-      <c r="X16" s="13"/>
-      <c r="Y16" s="13"/>
-      <c r="Z16" s="13"/>
-      <c r="AA16" s="13"/>
-      <c r="AB16" s="13"/>
-      <c r="AC16" s="13"/>
-      <c r="AD16" s="13"/>
-      <c r="AE16" s="13"/>
-      <c r="AF16" s="13"/>
-      <c r="AG16" s="13"/>
-      <c r="AH16" s="13"/>
-      <c r="AI16" s="13"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+      <c r="S16" s="16"/>
+      <c r="T16" s="16"/>
+      <c r="U16" s="16"/>
+      <c r="V16" s="16"/>
+      <c r="W16" s="16"/>
+      <c r="X16" s="16"/>
+      <c r="Y16" s="16"/>
+      <c r="Z16" s="16"/>
+      <c r="AA16" s="16"/>
+      <c r="AB16" s="16"/>
+      <c r="AC16" s="16"/>
+      <c r="AD16" s="16"/>
+      <c r="AE16" s="16"/>
+      <c r="AF16" s="16"/>
+      <c r="AG16" s="16"/>
+      <c r="AH16" s="16"/>
+      <c r="AI16" s="16"/>
     </row>
     <row r="17" s="3" customFormat="1" ht="14" customHeight="1" spans="1:35">
       <c r="A17" s="9">
@@ -2139,7 +2091,7 @@
         <v>36</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
@@ -2150,41 +2102,41 @@
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
       <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="13"/>
-      <c r="Q17" s="13"/>
-      <c r="R17" s="13"/>
-      <c r="S17" s="13"/>
-      <c r="T17" s="13"/>
-      <c r="U17" s="13"/>
-      <c r="V17" s="13"/>
-      <c r="W17" s="13"/>
-      <c r="X17" s="13"/>
-      <c r="Y17" s="13"/>
-      <c r="Z17" s="13"/>
-      <c r="AA17" s="13"/>
-      <c r="AB17" s="13"/>
-      <c r="AC17" s="13"/>
-      <c r="AD17" s="13"/>
-      <c r="AE17" s="13"/>
-      <c r="AF17" s="13"/>
-      <c r="AG17" s="13"/>
-      <c r="AH17" s="13"/>
-      <c r="AI17" s="13"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+      <c r="S17" s="16"/>
+      <c r="T17" s="16"/>
+      <c r="U17" s="16"/>
+      <c r="V17" s="16"/>
+      <c r="W17" s="16"/>
+      <c r="X17" s="16"/>
+      <c r="Y17" s="16"/>
+      <c r="Z17" s="16"/>
+      <c r="AA17" s="16"/>
+      <c r="AB17" s="16"/>
+      <c r="AC17" s="16"/>
+      <c r="AD17" s="16"/>
+      <c r="AE17" s="16"/>
+      <c r="AF17" s="16"/>
+      <c r="AG17" s="16"/>
+      <c r="AH17" s="16"/>
+      <c r="AI17" s="16"/>
     </row>
     <row r="18" s="3" customFormat="1" spans="1:35">
       <c r="A18" s="9">
         <v>14</v>
       </c>
       <c r="B18" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>39</v>
-      </c>
       <c r="D18" s="12" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
@@ -2195,41 +2147,41 @@
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>
       <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13"/>
-      <c r="Q18" s="13"/>
-      <c r="R18" s="13"/>
-      <c r="S18" s="13"/>
-      <c r="T18" s="13"/>
-      <c r="U18" s="13"/>
-      <c r="V18" s="13"/>
-      <c r="W18" s="13"/>
-      <c r="X18" s="13"/>
-      <c r="Y18" s="13"/>
-      <c r="Z18" s="13"/>
-      <c r="AA18" s="13"/>
-      <c r="AB18" s="13"/>
-      <c r="AC18" s="13"/>
-      <c r="AD18" s="13"/>
-      <c r="AE18" s="13"/>
-      <c r="AF18" s="13"/>
-      <c r="AG18" s="13"/>
-      <c r="AH18" s="13"/>
-      <c r="AI18" s="13"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="16"/>
+      <c r="R18" s="16"/>
+      <c r="S18" s="16"/>
+      <c r="T18" s="16"/>
+      <c r="U18" s="16"/>
+      <c r="V18" s="16"/>
+      <c r="W18" s="16"/>
+      <c r="X18" s="16"/>
+      <c r="Y18" s="16"/>
+      <c r="Z18" s="16"/>
+      <c r="AA18" s="16"/>
+      <c r="AB18" s="16"/>
+      <c r="AC18" s="16"/>
+      <c r="AD18" s="16"/>
+      <c r="AE18" s="16"/>
+      <c r="AF18" s="16"/>
+      <c r="AG18" s="16"/>
+      <c r="AH18" s="16"/>
+      <c r="AI18" s="16"/>
     </row>
     <row r="19" s="3" customFormat="1" spans="1:35">
       <c r="A19" s="9">
         <v>15</v>
       </c>
       <c r="B19" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="14" t="s">
-        <v>41</v>
-      </c>
       <c r="D19" s="12" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
@@ -2240,41 +2192,41 @@
       <c r="K19" s="13"/>
       <c r="L19" s="13"/>
       <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
-      <c r="P19" s="13"/>
-      <c r="Q19" s="13"/>
-      <c r="R19" s="13"/>
-      <c r="S19" s="13"/>
-      <c r="T19" s="13"/>
-      <c r="U19" s="13"/>
-      <c r="V19" s="13"/>
-      <c r="W19" s="13"/>
-      <c r="X19" s="13"/>
-      <c r="Y19" s="13"/>
-      <c r="Z19" s="13"/>
-      <c r="AA19" s="13"/>
-      <c r="AB19" s="13"/>
-      <c r="AC19" s="13"/>
-      <c r="AD19" s="13"/>
-      <c r="AE19" s="13"/>
-      <c r="AF19" s="13"/>
-      <c r="AG19" s="13"/>
-      <c r="AH19" s="13"/>
-      <c r="AI19" s="13"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="16"/>
+      <c r="R19" s="16"/>
+      <c r="S19" s="16"/>
+      <c r="T19" s="16"/>
+      <c r="U19" s="16"/>
+      <c r="V19" s="16"/>
+      <c r="W19" s="16"/>
+      <c r="X19" s="16"/>
+      <c r="Y19" s="16"/>
+      <c r="Z19" s="16"/>
+      <c r="AA19" s="16"/>
+      <c r="AB19" s="16"/>
+      <c r="AC19" s="16"/>
+      <c r="AD19" s="16"/>
+      <c r="AE19" s="16"/>
+      <c r="AF19" s="16"/>
+      <c r="AG19" s="16"/>
+      <c r="AH19" s="16"/>
+      <c r="AI19" s="16"/>
     </row>
     <row r="20" s="3" customFormat="1" spans="1:35">
       <c r="A20" s="9">
         <v>16</v>
       </c>
       <c r="B20" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="12" t="s">
-        <v>43</v>
-      </c>
       <c r="D20" s="12" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
@@ -2285,41 +2237,41 @@
       <c r="K20" s="13"/>
       <c r="L20" s="13"/>
       <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="13"/>
-      <c r="R20" s="13"/>
-      <c r="S20" s="13"/>
-      <c r="T20" s="13"/>
-      <c r="U20" s="13"/>
-      <c r="V20" s="13"/>
-      <c r="W20" s="13"/>
-      <c r="X20" s="13"/>
-      <c r="Y20" s="13"/>
-      <c r="Z20" s="13"/>
-      <c r="AA20" s="13"/>
-      <c r="AB20" s="13"/>
-      <c r="AC20" s="13"/>
-      <c r="AD20" s="13"/>
-      <c r="AE20" s="13"/>
-      <c r="AF20" s="13"/>
-      <c r="AG20" s="13"/>
-      <c r="AH20" s="13"/>
-      <c r="AI20" s="13"/>
-    </row>
-    <row r="21" spans="1:35">
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="16"/>
+      <c r="R20" s="16"/>
+      <c r="S20" s="16"/>
+      <c r="T20" s="16"/>
+      <c r="U20" s="16"/>
+      <c r="V20" s="16"/>
+      <c r="W20" s="16"/>
+      <c r="X20" s="16"/>
+      <c r="Y20" s="16"/>
+      <c r="Z20" s="16"/>
+      <c r="AA20" s="16"/>
+      <c r="AB20" s="16"/>
+      <c r="AC20" s="16"/>
+      <c r="AD20" s="16"/>
+      <c r="AE20" s="16"/>
+      <c r="AF20" s="16"/>
+      <c r="AG20" s="16"/>
+      <c r="AH20" s="16"/>
+      <c r="AI20" s="16"/>
+    </row>
+    <row r="21" s="3" customFormat="1" spans="1:35">
       <c r="A21" s="9">
         <v>17</v>
       </c>
       <c r="B21" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="12" t="s">
-        <v>45</v>
-      </c>
       <c r="D21" s="12" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
@@ -2330,41 +2282,41 @@
       <c r="K21" s="13"/>
       <c r="L21" s="13"/>
       <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="13"/>
-      <c r="Q21" s="13"/>
-      <c r="R21" s="13"/>
-      <c r="S21" s="13"/>
-      <c r="T21" s="13"/>
-      <c r="U21" s="13"/>
-      <c r="V21" s="13"/>
-      <c r="W21" s="13"/>
-      <c r="X21" s="13"/>
-      <c r="Y21" s="13"/>
-      <c r="Z21" s="13"/>
-      <c r="AA21" s="13"/>
-      <c r="AB21" s="13"/>
-      <c r="AC21" s="13"/>
-      <c r="AD21" s="13"/>
-      <c r="AE21" s="13"/>
-      <c r="AF21" s="13"/>
-      <c r="AG21" s="13"/>
-      <c r="AH21" s="13"/>
-      <c r="AI21" s="13"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="16"/>
+      <c r="Q21" s="16"/>
+      <c r="R21" s="16"/>
+      <c r="S21" s="16"/>
+      <c r="T21" s="16"/>
+      <c r="U21" s="16"/>
+      <c r="V21" s="16"/>
+      <c r="W21" s="16"/>
+      <c r="X21" s="16"/>
+      <c r="Y21" s="16"/>
+      <c r="Z21" s="16"/>
+      <c r="AA21" s="16"/>
+      <c r="AB21" s="16"/>
+      <c r="AC21" s="16"/>
+      <c r="AD21" s="16"/>
+      <c r="AE21" s="16"/>
+      <c r="AF21" s="16"/>
+      <c r="AG21" s="16"/>
+      <c r="AH21" s="16"/>
+      <c r="AI21" s="16"/>
     </row>
     <row r="22" spans="1:35">
       <c r="A22" s="9">
         <v>18</v>
       </c>
       <c r="B22" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="12" t="s">
-        <v>47</v>
-      </c>
       <c r="D22" s="12" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
@@ -2375,41 +2327,41 @@
       <c r="K22" s="13"/>
       <c r="L22" s="13"/>
       <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13"/>
-      <c r="Q22" s="13"/>
-      <c r="R22" s="13"/>
-      <c r="S22" s="13"/>
-      <c r="T22" s="13"/>
-      <c r="U22" s="13"/>
-      <c r="V22" s="13"/>
-      <c r="W22" s="13"/>
-      <c r="X22" s="13"/>
-      <c r="Y22" s="13"/>
-      <c r="Z22" s="13"/>
-      <c r="AA22" s="13"/>
-      <c r="AB22" s="13"/>
-      <c r="AC22" s="13"/>
-      <c r="AD22" s="13"/>
-      <c r="AE22" s="13"/>
-      <c r="AF22" s="13"/>
-      <c r="AG22" s="13"/>
-      <c r="AH22" s="13"/>
-      <c r="AI22" s="13"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="16"/>
+      <c r="P22" s="16"/>
+      <c r="Q22" s="16"/>
+      <c r="R22" s="16"/>
+      <c r="S22" s="16"/>
+      <c r="T22" s="16"/>
+      <c r="U22" s="16"/>
+      <c r="V22" s="16"/>
+      <c r="W22" s="16"/>
+      <c r="X22" s="16"/>
+      <c r="Y22" s="16"/>
+      <c r="Z22" s="16"/>
+      <c r="AA22" s="16"/>
+      <c r="AB22" s="16"/>
+      <c r="AC22" s="16"/>
+      <c r="AD22" s="16"/>
+      <c r="AE22" s="16"/>
+      <c r="AF22" s="16"/>
+      <c r="AG22" s="16"/>
+      <c r="AH22" s="16"/>
+      <c r="AI22" s="16"/>
     </row>
     <row r="23" spans="1:35">
       <c r="A23" s="9">
         <v>19</v>
       </c>
       <c r="B23" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>49</v>
-      </c>
       <c r="D23" s="12" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="E23" s="13"/>
       <c r="F23" s="13"/>
@@ -2420,41 +2372,41 @@
       <c r="K23" s="13"/>
       <c r="L23" s="13"/>
       <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
-      <c r="Q23" s="13"/>
-      <c r="R23" s="13"/>
-      <c r="S23" s="13"/>
-      <c r="T23" s="13"/>
-      <c r="U23" s="13"/>
-      <c r="V23" s="13"/>
-      <c r="W23" s="13"/>
-      <c r="X23" s="13"/>
-      <c r="Y23" s="13"/>
-      <c r="Z23" s="13"/>
-      <c r="AA23" s="13"/>
-      <c r="AB23" s="13"/>
-      <c r="AC23" s="13"/>
-      <c r="AD23" s="13"/>
-      <c r="AE23" s="13"/>
-      <c r="AF23" s="13"/>
-      <c r="AG23" s="13"/>
-      <c r="AH23" s="13"/>
-      <c r="AI23" s="13"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="16"/>
+      <c r="Q23" s="16"/>
+      <c r="R23" s="16"/>
+      <c r="S23" s="16"/>
+      <c r="T23" s="16"/>
+      <c r="U23" s="16"/>
+      <c r="V23" s="16"/>
+      <c r="W23" s="16"/>
+      <c r="X23" s="16"/>
+      <c r="Y23" s="16"/>
+      <c r="Z23" s="16"/>
+      <c r="AA23" s="16"/>
+      <c r="AB23" s="16"/>
+      <c r="AC23" s="16"/>
+      <c r="AD23" s="16"/>
+      <c r="AE23" s="16"/>
+      <c r="AF23" s="16"/>
+      <c r="AG23" s="16"/>
+      <c r="AH23" s="16"/>
+      <c r="AI23" s="16"/>
     </row>
     <row r="24" spans="1:35">
       <c r="A24" s="9">
         <v>20</v>
       </c>
       <c r="B24" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>51</v>
-      </c>
       <c r="D24" s="12" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="E24" s="13"/>
       <c r="F24" s="13"/>
@@ -2465,41 +2417,41 @@
       <c r="K24" s="13"/>
       <c r="L24" s="13"/>
       <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="13"/>
-      <c r="P24" s="13"/>
-      <c r="Q24" s="13"/>
-      <c r="R24" s="13"/>
-      <c r="S24" s="13"/>
-      <c r="T24" s="13"/>
-      <c r="U24" s="13"/>
-      <c r="V24" s="13"/>
-      <c r="W24" s="13"/>
-      <c r="X24" s="13"/>
-      <c r="Y24" s="13"/>
-      <c r="Z24" s="13"/>
-      <c r="AA24" s="13"/>
-      <c r="AB24" s="13"/>
-      <c r="AC24" s="13"/>
-      <c r="AD24" s="13"/>
-      <c r="AE24" s="13"/>
-      <c r="AF24" s="13"/>
-      <c r="AG24" s="13"/>
-      <c r="AH24" s="13"/>
-      <c r="AI24" s="13"/>
+      <c r="N24" s="16"/>
+      <c r="O24" s="16"/>
+      <c r="P24" s="16"/>
+      <c r="Q24" s="16"/>
+      <c r="R24" s="16"/>
+      <c r="S24" s="16"/>
+      <c r="T24" s="16"/>
+      <c r="U24" s="16"/>
+      <c r="V24" s="16"/>
+      <c r="W24" s="16"/>
+      <c r="X24" s="16"/>
+      <c r="Y24" s="16"/>
+      <c r="Z24" s="16"/>
+      <c r="AA24" s="16"/>
+      <c r="AB24" s="16"/>
+      <c r="AC24" s="16"/>
+      <c r="AD24" s="16"/>
+      <c r="AE24" s="16"/>
+      <c r="AF24" s="16"/>
+      <c r="AG24" s="16"/>
+      <c r="AH24" s="16"/>
+      <c r="AI24" s="16"/>
     </row>
     <row r="25" spans="1:35">
       <c r="A25" s="9">
         <v>21</v>
       </c>
       <c r="B25" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="12" t="s">
-        <v>53</v>
-      </c>
       <c r="D25" s="12" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
@@ -2510,41 +2462,41 @@
       <c r="K25" s="13"/>
       <c r="L25" s="13"/>
       <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="13"/>
-      <c r="P25" s="13"/>
-      <c r="Q25" s="13"/>
-      <c r="R25" s="13"/>
-      <c r="S25" s="13"/>
-      <c r="T25" s="13"/>
-      <c r="U25" s="13"/>
-      <c r="V25" s="13"/>
-      <c r="W25" s="13"/>
-      <c r="X25" s="13"/>
-      <c r="Y25" s="13"/>
-      <c r="Z25" s="13"/>
-      <c r="AA25" s="13"/>
-      <c r="AB25" s="13"/>
-      <c r="AC25" s="13"/>
-      <c r="AD25" s="13"/>
-      <c r="AE25" s="13"/>
-      <c r="AF25" s="13"/>
-      <c r="AG25" s="13"/>
-      <c r="AH25" s="13"/>
-      <c r="AI25" s="13"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="16"/>
+      <c r="Q25" s="16"/>
+      <c r="R25" s="16"/>
+      <c r="S25" s="16"/>
+      <c r="T25" s="16"/>
+      <c r="U25" s="16"/>
+      <c r="V25" s="16"/>
+      <c r="W25" s="16"/>
+      <c r="X25" s="16"/>
+      <c r="Y25" s="16"/>
+      <c r="Z25" s="16"/>
+      <c r="AA25" s="16"/>
+      <c r="AB25" s="16"/>
+      <c r="AC25" s="16"/>
+      <c r="AD25" s="16"/>
+      <c r="AE25" s="16"/>
+      <c r="AF25" s="16"/>
+      <c r="AG25" s="16"/>
+      <c r="AH25" s="16"/>
+      <c r="AI25" s="16"/>
     </row>
     <row r="26" spans="1:35">
       <c r="A26" s="9">
         <v>22</v>
       </c>
       <c r="B26" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="12" t="s">
-        <v>55</v>
-      </c>
       <c r="D26" s="12" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
@@ -2555,41 +2507,41 @@
       <c r="K26" s="13"/>
       <c r="L26" s="13"/>
       <c r="M26" s="13"/>
-      <c r="N26" s="13"/>
-      <c r="O26" s="13"/>
-      <c r="P26" s="13"/>
-      <c r="Q26" s="13"/>
-      <c r="R26" s="13"/>
-      <c r="S26" s="13"/>
-      <c r="T26" s="13"/>
-      <c r="U26" s="13"/>
-      <c r="V26" s="13"/>
-      <c r="W26" s="13"/>
-      <c r="X26" s="13"/>
-      <c r="Y26" s="13"/>
-      <c r="Z26" s="13"/>
-      <c r="AA26" s="13"/>
-      <c r="AB26" s="13"/>
-      <c r="AC26" s="13"/>
-      <c r="AD26" s="13"/>
-      <c r="AE26" s="13"/>
-      <c r="AF26" s="13"/>
-      <c r="AG26" s="13"/>
-      <c r="AH26" s="13"/>
-      <c r="AI26" s="13"/>
+      <c r="N26" s="16"/>
+      <c r="O26" s="16"/>
+      <c r="P26" s="16"/>
+      <c r="Q26" s="16"/>
+      <c r="R26" s="16"/>
+      <c r="S26" s="16"/>
+      <c r="T26" s="16"/>
+      <c r="U26" s="16"/>
+      <c r="V26" s="16"/>
+      <c r="W26" s="16"/>
+      <c r="X26" s="16"/>
+      <c r="Y26" s="16"/>
+      <c r="Z26" s="16"/>
+      <c r="AA26" s="16"/>
+      <c r="AB26" s="16"/>
+      <c r="AC26" s="16"/>
+      <c r="AD26" s="16"/>
+      <c r="AE26" s="16"/>
+      <c r="AF26" s="16"/>
+      <c r="AG26" s="16"/>
+      <c r="AH26" s="16"/>
+      <c r="AI26" s="16"/>
     </row>
     <row r="27" spans="1:35">
       <c r="A27" s="9">
         <v>23</v>
       </c>
       <c r="B27" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C27" s="12" t="s">
-        <v>57</v>
-      </c>
       <c r="D27" s="12" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E27" s="13"/>
       <c r="F27" s="13"/>
@@ -2600,377 +2552,28 @@
       <c r="K27" s="13"/>
       <c r="L27" s="13"/>
       <c r="M27" s="13"/>
-      <c r="N27" s="13"/>
-      <c r="O27" s="13"/>
-      <c r="P27" s="13"/>
-      <c r="Q27" s="13"/>
-      <c r="R27" s="13"/>
-      <c r="S27" s="13"/>
-      <c r="T27" s="13"/>
-      <c r="U27" s="13"/>
-      <c r="V27" s="13"/>
-      <c r="W27" s="13"/>
-      <c r="X27" s="13"/>
-      <c r="Y27" s="13"/>
-      <c r="Z27" s="13"/>
-      <c r="AA27" s="13"/>
-      <c r="AB27" s="13"/>
-      <c r="AC27" s="13"/>
-      <c r="AD27" s="13"/>
-      <c r="AE27" s="13"/>
-      <c r="AF27" s="13"/>
-      <c r="AG27" s="13"/>
-      <c r="AH27" s="13"/>
-      <c r="AI27" s="13"/>
-    </row>
-    <row r="28" spans="1:35">
-      <c r="A28" s="9">
-        <v>24</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="13"/>
-      <c r="O28" s="13"/>
-      <c r="P28" s="13"/>
-      <c r="Q28" s="13"/>
-      <c r="R28" s="13"/>
-      <c r="S28" s="13"/>
-      <c r="T28" s="13"/>
-      <c r="U28" s="13"/>
-      <c r="V28" s="13"/>
-      <c r="W28" s="13"/>
-      <c r="X28" s="13"/>
-      <c r="Y28" s="13"/>
-      <c r="Z28" s="13"/>
-      <c r="AA28" s="13"/>
-      <c r="AB28" s="13"/>
-      <c r="AC28" s="13"/>
-      <c r="AD28" s="13"/>
-      <c r="AE28" s="13"/>
-      <c r="AF28" s="13"/>
-      <c r="AG28" s="13"/>
-      <c r="AH28" s="13"/>
-      <c r="AI28" s="13"/>
-    </row>
-    <row r="29" spans="1:35">
-      <c r="A29" s="9">
-        <v>25</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="13"/>
-      <c r="N29" s="13"/>
-      <c r="O29" s="13"/>
-      <c r="P29" s="13"/>
-      <c r="Q29" s="13"/>
-      <c r="R29" s="13"/>
-      <c r="S29" s="13"/>
-      <c r="T29" s="13"/>
-      <c r="U29" s="13"/>
-      <c r="V29" s="13"/>
-      <c r="W29" s="13"/>
-      <c r="X29" s="13"/>
-      <c r="Y29" s="13"/>
-      <c r="Z29" s="13"/>
-      <c r="AA29" s="13"/>
-      <c r="AB29" s="13"/>
-      <c r="AC29" s="13"/>
-      <c r="AD29" s="13"/>
-      <c r="AE29" s="13"/>
-      <c r="AF29" s="13"/>
-      <c r="AG29" s="13"/>
-      <c r="AH29" s="13"/>
-      <c r="AI29" s="13"/>
-    </row>
-    <row r="30" spans="1:35">
-      <c r="A30" s="9"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
-      <c r="M30" s="13"/>
-      <c r="N30" s="13"/>
-      <c r="O30" s="13"/>
-      <c r="P30" s="13"/>
-      <c r="Q30" s="13"/>
-      <c r="R30" s="13"/>
-      <c r="S30" s="13"/>
-      <c r="T30" s="13"/>
-      <c r="U30" s="13"/>
-      <c r="V30" s="13"/>
-      <c r="W30" s="13"/>
-      <c r="X30" s="13"/>
-      <c r="Y30" s="13"/>
-      <c r="Z30" s="13"/>
-      <c r="AA30" s="13"/>
-      <c r="AB30" s="13"/>
-      <c r="AC30" s="13"/>
-      <c r="AD30" s="13"/>
-      <c r="AE30" s="13"/>
-      <c r="AF30" s="13"/>
-      <c r="AG30" s="13"/>
-      <c r="AH30" s="13"/>
-      <c r="AI30" s="13"/>
-    </row>
-    <row r="31" spans="1:35">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="13"/>
-      <c r="N31" s="13"/>
-      <c r="O31" s="13"/>
-      <c r="P31" s="13"/>
-      <c r="Q31" s="13"/>
-      <c r="R31" s="13"/>
-      <c r="S31" s="13"/>
-      <c r="T31" s="13"/>
-      <c r="U31" s="13"/>
-      <c r="V31" s="13"/>
-      <c r="W31" s="13"/>
-      <c r="X31" s="13"/>
-      <c r="Y31" s="13"/>
-      <c r="Z31" s="13"/>
-      <c r="AA31" s="13"/>
-      <c r="AB31" s="13"/>
-      <c r="AC31" s="13"/>
-      <c r="AD31" s="13"/>
-      <c r="AE31" s="13"/>
-      <c r="AF31" s="13"/>
-      <c r="AG31" s="13"/>
-      <c r="AH31" s="13"/>
-      <c r="AI31" s="13"/>
-    </row>
-    <row r="32" spans="1:35">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="13"/>
-      <c r="L32" s="13"/>
-      <c r="M32" s="13"/>
-      <c r="N32" s="13"/>
-      <c r="O32" s="13"/>
-      <c r="P32" s="13"/>
-      <c r="Q32" s="13"/>
-      <c r="R32" s="13"/>
-      <c r="S32" s="13"/>
-      <c r="T32" s="13"/>
-      <c r="U32" s="13"/>
-      <c r="V32" s="13"/>
-      <c r="W32" s="13"/>
-      <c r="X32" s="13"/>
-      <c r="Y32" s="13"/>
-      <c r="Z32" s="13"/>
-      <c r="AA32" s="13"/>
-      <c r="AB32" s="13"/>
-      <c r="AC32" s="13"/>
-      <c r="AD32" s="13"/>
-      <c r="AE32" s="13"/>
-      <c r="AF32" s="13"/>
-      <c r="AG32" s="13"/>
-      <c r="AH32" s="13"/>
-      <c r="AI32" s="13"/>
-    </row>
-    <row r="33" spans="1:35">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="13"/>
-      <c r="L33" s="13"/>
-      <c r="M33" s="13"/>
-      <c r="N33" s="13"/>
-      <c r="O33" s="13"/>
-      <c r="P33" s="13"/>
-      <c r="Q33" s="13"/>
-      <c r="R33" s="13"/>
-      <c r="S33" s="13"/>
-      <c r="T33" s="13"/>
-      <c r="U33" s="13"/>
-      <c r="V33" s="13"/>
-      <c r="W33" s="13"/>
-      <c r="X33" s="13"/>
-      <c r="Y33" s="13"/>
-      <c r="Z33" s="13"/>
-      <c r="AA33" s="13"/>
-      <c r="AB33" s="13"/>
-      <c r="AC33" s="13"/>
-      <c r="AD33" s="13"/>
-      <c r="AE33" s="13"/>
-      <c r="AF33" s="13"/>
-      <c r="AG33" s="13"/>
-      <c r="AH33" s="13"/>
-      <c r="AI33" s="13"/>
-    </row>
-    <row r="34" spans="1:35">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13"/>
-      <c r="J34" s="13"/>
-      <c r="K34" s="13"/>
-      <c r="L34" s="13"/>
-      <c r="M34" s="13"/>
-      <c r="N34" s="13"/>
-      <c r="O34" s="13"/>
-      <c r="P34" s="13"/>
-      <c r="Q34" s="13"/>
-      <c r="R34" s="13"/>
-      <c r="S34" s="13"/>
-      <c r="T34" s="13"/>
-      <c r="U34" s="13"/>
-      <c r="V34" s="13"/>
-      <c r="W34" s="13"/>
-      <c r="X34" s="13"/>
-      <c r="Y34" s="13"/>
-      <c r="Z34" s="13"/>
-      <c r="AA34" s="13"/>
-      <c r="AB34" s="13"/>
-      <c r="AC34" s="13"/>
-      <c r="AD34" s="13"/>
-      <c r="AE34" s="13"/>
-      <c r="AF34" s="13"/>
-      <c r="AG34" s="13"/>
-      <c r="AH34" s="13"/>
-      <c r="AI34" s="13"/>
-    </row>
-    <row r="35" spans="1:35">
-      <c r="A35" s="12"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="13"/>
-      <c r="K35" s="13"/>
-      <c r="L35" s="13"/>
-      <c r="M35" s="13"/>
-      <c r="N35" s="13"/>
-      <c r="O35" s="13"/>
-      <c r="P35" s="13"/>
-      <c r="Q35" s="13"/>
-      <c r="R35" s="13"/>
-      <c r="S35" s="13"/>
-      <c r="T35" s="13"/>
-      <c r="U35" s="13"/>
-      <c r="V35" s="13"/>
-      <c r="W35" s="13"/>
-      <c r="X35" s="13"/>
-      <c r="Y35" s="13"/>
-      <c r="Z35" s="13"/>
-      <c r="AA35" s="13"/>
-      <c r="AB35" s="13"/>
-      <c r="AC35" s="13"/>
-      <c r="AD35" s="13"/>
-      <c r="AE35" s="13"/>
-      <c r="AF35" s="13"/>
-      <c r="AG35" s="13"/>
-      <c r="AH35" s="13"/>
-      <c r="AI35" s="13"/>
-    </row>
-    <row r="36" spans="1:35">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="13"/>
-      <c r="K36" s="13"/>
-      <c r="L36" s="13"/>
-      <c r="M36" s="13"/>
-      <c r="N36" s="13"/>
-      <c r="O36" s="13"/>
-      <c r="P36" s="13"/>
-      <c r="Q36" s="13"/>
-      <c r="R36" s="13"/>
-      <c r="S36" s="13"/>
-      <c r="T36" s="13"/>
-      <c r="U36" s="13"/>
-      <c r="V36" s="13"/>
-      <c r="W36" s="13"/>
-      <c r="X36" s="13"/>
-      <c r="Y36" s="13"/>
-      <c r="Z36" s="13"/>
-      <c r="AA36" s="13"/>
-      <c r="AB36" s="13"/>
-      <c r="AC36" s="13"/>
-      <c r="AD36" s="13"/>
-      <c r="AE36" s="13"/>
-      <c r="AF36" s="13"/>
-      <c r="AG36" s="13"/>
-      <c r="AH36" s="13"/>
-      <c r="AI36" s="13"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="16"/>
+      <c r="Q27" s="16"/>
+      <c r="R27" s="16"/>
+      <c r="S27" s="16"/>
+      <c r="T27" s="16"/>
+      <c r="U27" s="16"/>
+      <c r="V27" s="16"/>
+      <c r="W27" s="16"/>
+      <c r="X27" s="16"/>
+      <c r="Y27" s="16"/>
+      <c r="Z27" s="16"/>
+      <c r="AA27" s="16"/>
+      <c r="AB27" s="16"/>
+      <c r="AC27" s="16"/>
+      <c r="AD27" s="16"/>
+      <c r="AE27" s="16"/>
+      <c r="AF27" s="16"/>
+      <c r="AG27" s="16"/>
+      <c r="AH27" s="16"/>
+      <c r="AI27" s="16"/>
     </row>
   </sheetData>
   <sortState ref="B5:D36">

</xml_diff>